<commit_message>
Update stiffness test data.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Tests/Stiffness Measurements.xlsx
+++ b/design_spreadsheets/Tests/Stiffness Measurements.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bottom of travel" sheetId="1" r:id="rId1"/>
+    <sheet name="top of travel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>weight in lb</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>2 sigma minus</t>
+  </si>
+  <si>
+    <t>yellow cells are differential deflections between 10lb and 20lb loadings, i.e. takes up any slop or geometric error, should be better measure of F=kx stiffness</t>
   </si>
 </sst>
 </file>
@@ -70,12 +73,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G36:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,22 +415,22 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B7" si="0">A2*0.4563</f>
+        <f t="shared" ref="B2:B3" si="0">A2*0.4563</f>
         <v>4.5629999999999997</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C7" si="1">9.8*B2</f>
+        <f t="shared" ref="C2:C3" si="1">9.8*B2</f>
         <v>44.717399999999998</v>
       </c>
       <c r="D2">
         <v>41</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E7" si="2">D2/1000 *25.4</f>
+        <f t="shared" ref="E2:E3" si="2">D2/1000 *25.4</f>
         <v>1.0413999999999999</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F7" si="3">C2/E2</f>
+        <f t="shared" ref="F2:F3" si="3">C2/E2</f>
         <v>42.939696562319959</v>
       </c>
     </row>
@@ -449,139 +459,477 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>4.5629999999999997</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
-        <v>44.717399999999998</v>
-      </c>
-      <c r="D4">
-        <v>38</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="2"/>
-        <v>0.96519999999999995</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
-        <v>46.329672606713636</v>
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4" si="4">A4*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4" si="5">9.8*B4</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <f>D3-D2</f>
+        <v>31</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4" si="6">D4/1000 *25.4</f>
+        <v>0.78739999999999999</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4" si="7">C4/E4</f>
+        <v>56.791211582423166</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>9.1259999999999994</v>
+        <f>A5*0.4563</f>
+        <v>4.5629999999999997</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>89.434799999999996</v>
+        <f>9.8*B5</f>
+        <v>44.717399999999998</v>
       </c>
       <c r="D5">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>1.8287999999999998</v>
+        <f>D5/1000 *25.4</f>
+        <v>0.96519999999999995</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
-        <v>48.903543307086615</v>
+        <f>C5/E5</f>
+        <v>46.329672606713636</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B6">
+        <f>A6*0.4563</f>
+        <v>9.1259999999999994</v>
+      </c>
+      <c r="C6">
+        <f>9.8*B6</f>
+        <v>89.434799999999996</v>
+      </c>
+      <c r="D6">
+        <v>72</v>
+      </c>
+      <c r="E6">
+        <f>D6/1000 *25.4</f>
+        <v>1.8287999999999998</v>
+      </c>
+      <c r="F6">
+        <f>C6/E6</f>
+        <v>48.903543307086615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <f>A7*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C7" s="1">
+        <f>9.8*B7</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D7" s="1">
+        <f>D6-D5</f>
+        <v>34</v>
+      </c>
+      <c r="E7" s="1">
+        <f>D7/1000 *25.4</f>
+        <v>0.86360000000000003</v>
+      </c>
+      <c r="F7" s="1">
+        <f>C7/E7</f>
+        <v>51.780222325150525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>A8*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C8">
+        <f>9.8*B8</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D8">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <f>D8/1000 *25.4</f>
+        <v>0.91439999999999988</v>
+      </c>
+      <c r="F8">
+        <f>C8/E8</f>
+        <v>48.903543307086615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <f>A9*0.4563</f>
+        <v>9.1259999999999994</v>
+      </c>
+      <c r="C9">
+        <f>9.8*B9</f>
+        <v>89.434799999999996</v>
+      </c>
+      <c r="D9">
+        <v>68</v>
+      </c>
+      <c r="E9">
+        <f>D9/1000 *25.4</f>
+        <v>1.7272000000000001</v>
+      </c>
+      <c r="F9">
+        <f>C9/E9</f>
+        <v>51.780222325150525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <f>A10*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C10" s="1">
+        <f>9.8*B10</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D10" s="1">
+        <f>D9-D8</f>
+        <v>32</v>
+      </c>
+      <c r="E10" s="1">
+        <f>D10/1000 *25.4</f>
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="F10" s="1">
+        <f>C10/E10</f>
+        <v>55.016486220472437</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>AVERAGE(F2:F9)</f>
+        <v>49.541456915377211</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <f>F12+F13</f>
+        <v>53.642026272566746</v>
+      </c>
+      <c r="K12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f>F12+2*F13</f>
+        <v>57.742595629756288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f>_xlfn.STDEV.S(F2:F9)</f>
+        <v>4.1005693571895376</v>
+      </c>
+      <c r="H13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <f>F12-F13</f>
+        <v>45.440887558187676</v>
+      </c>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <f>F12-2*F13</f>
+        <v>41.340318200998134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <f>A2*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C2">
+        <f>9.8*B2</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D2">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <f>D2/1000*25.4</f>
+        <v>0.73660000000000003</v>
+      </c>
+      <c r="F2">
+        <f>C2/E2</f>
+        <v>60.707846863969586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">A3*0.4563</f>
+        <v>9.1259999999999994</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="1">9.8*B3</f>
+        <v>89.434799999999996</v>
+      </c>
+      <c r="D3">
+        <v>62</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E4" si="2">D3/1000*25.4</f>
+        <v>1.5748</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3" si="3">C3/E3</f>
+        <v>56.791211582423166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
         <f t="shared" si="0"/>
         <v>4.5629999999999997</v>
       </c>
+      <c r="C4" s="1">
+        <f t="shared" si="1"/>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <f>D3-D2</f>
+        <v>33</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83819999999999995</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4" si="4">C4/E4</f>
+        <v>53.349319971367215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <f>A5*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C5">
+        <f>9.8*B5</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <f>D5/1000*25.4</f>
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="F5">
+        <f>C5/E5</f>
+        <v>55.016486220472437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <f>A6*0.4563</f>
+        <v>9.1259999999999994</v>
+      </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>44.717399999999998</v>
+        <f>9.8*B6</f>
+        <v>89.434799999999996</v>
       </c>
       <c r="D6">
-        <v>36</v>
+        <v>70.5</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>0.91439999999999988</v>
+        <f>D6/1000*25.4</f>
+        <v>1.7906999999999997</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
-        <v>48.903543307086615</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <f>C6/E6</f>
+        <v>49.944044228513995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <f>A7*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C7" s="1">
+        <f>9.8*B7</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D7" s="1">
+        <f>D6-D5</f>
+        <v>38.5</v>
+      </c>
+      <c r="E7" s="1">
+        <f>D7/1000*25.4</f>
+        <v>0.97789999999999988</v>
+      </c>
+      <c r="F7" s="1">
+        <f>C7/E7</f>
+        <v>45.727988546886188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>A8*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C8">
+        <f>9.8*B8</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D8">
+        <v>27</v>
+      </c>
+      <c r="E8">
+        <f>D8/1000*25.4</f>
+        <v>0.68579999999999997</v>
+      </c>
+      <c r="F8">
+        <f>C8/E8</f>
+        <v>65.204724409448815</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>20</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
+      <c r="B9">
+        <f>A9*0.4563</f>
         <v>9.1259999999999994</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
+      <c r="C9">
+        <f>9.8*B9</f>
         <v>89.434799999999996</v>
       </c>
-      <c r="D7">
-        <v>68</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>1.7272000000000001</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>51.780222325150525</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <f>D9/1000*25.4</f>
+        <v>1.6255999999999999</v>
+      </c>
       <c r="F9">
-        <f>AVERAGE(F2:F7)</f>
-        <v>47.960036902573989</v>
-      </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <f>F9+F10</f>
-        <v>50.964245102354205</v>
-      </c>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9">
-        <f>F9+2*F10</f>
-        <v>53.968453302134421</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F10">
-        <f>_xlfn.STDEV.S(F2:F7)</f>
-        <v>3.004208199780217</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10">
-        <f>F9-F10</f>
-        <v>44.955828702793774</v>
-      </c>
-      <c r="K10" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10">
-        <f>F9-2*F10</f>
-        <v>41.951620503013558</v>
+        <f>C9/E9</f>
+        <v>55.016486220472437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <f>A10*0.4563</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="C10" s="1">
+        <f>9.8*B10</f>
+        <v>44.717399999999998</v>
+      </c>
+      <c r="D10" s="1">
+        <f>D9-D8</f>
+        <v>37</v>
+      </c>
+      <c r="E10" s="1">
+        <f>D10/1000*25.4</f>
+        <v>0.93979999999999986</v>
+      </c>
+      <c r="F10" s="1">
+        <f>C10/E10</f>
+        <v>47.581825920408605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculate summary statistics and prediction error for stiffness measurements.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Tests/Stiffness Measurements.xlsx
+++ b/design_spreadsheets/Tests/Stiffness Measurements.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>weight in lb</t>
   </si>
@@ -36,35 +36,47 @@
     <t>weight in N</t>
   </si>
   <si>
-    <t>deflection in thou</t>
-  </si>
-  <si>
     <t>deflection in mm</t>
   </si>
   <si>
     <t>stiffness (N/mm)</t>
   </si>
   <si>
-    <t>1 sigma plus</t>
-  </si>
-  <si>
-    <t>1 sigma minus</t>
-  </si>
-  <si>
-    <t>2 sigma plus</t>
-  </si>
-  <si>
-    <t>2 sigma minus</t>
-  </si>
-  <si>
     <t>yellow cells are differential deflections between 10lb and 20lb loadings, i.e. takes up any slop or geometric error, should be better measure of F=kx stiffness</t>
+  </si>
+  <si>
+    <t>Mean measured stiffness (N/mm)</t>
+  </si>
+  <si>
+    <t>deflection in 0.001"</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Stdev measured stiffness (N/mm)</t>
+  </si>
+  <si>
+    <t>95% confidence interval (N/mm)</t>
+  </si>
+  <si>
+    <t>Upper bound (N/mm)</t>
+  </si>
+  <si>
+    <t>Lower bound (N/mm)</t>
+  </si>
+  <si>
+    <t>Predicted stiffness from error budget (N/mm)</t>
+  </si>
+  <si>
+    <t>Prediction relative error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,8 +84,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -99,9 +132,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,35 +418,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G36:G37"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -433,8 +481,15 @@
         <f t="shared" ref="F2:F3" si="3">C2/E2</f>
         <v>42.939696562319959</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(F2:F10)</f>
+        <v>50.149793504832232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -457,8 +512,15 @@
         <f t="shared" si="3"/>
         <v>48.903543307086615</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <f>_xlfn.STDEV.S(F2:F10)</f>
+        <v>4.2477636558675842</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>10</v>
       </c>
@@ -482,65 +544,86 @@
         <f t="shared" ref="F4" si="7">C4/E4</f>
         <v>56.791211582423166</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <f>_xlfn.CONFIDENCE.NORM(0.05,I3,COUNT(F2:F10))</f>
+        <v>2.7751545934462185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5">
-        <f>A5*0.4563</f>
+        <f t="shared" ref="B5:B10" si="8">A5*0.4563</f>
         <v>4.5629999999999997</v>
       </c>
       <c r="C5">
-        <f>9.8*B5</f>
+        <f t="shared" ref="C5:C10" si="9">9.8*B5</f>
         <v>44.717399999999998</v>
       </c>
       <c r="D5">
         <v>38</v>
       </c>
       <c r="E5">
-        <f>D5/1000 *25.4</f>
+        <f t="shared" ref="E5:E10" si="10">D5/1000 *25.4</f>
         <v>0.96519999999999995</v>
       </c>
       <c r="F5">
-        <f>C5/E5</f>
+        <f t="shared" ref="F5:F10" si="11">C5/E5</f>
         <v>46.329672606713636</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <f>I2+I4</f>
+        <v>52.924948098278449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
       <c r="B6">
-        <f>A6*0.4563</f>
+        <f t="shared" si="8"/>
         <v>9.1259999999999994</v>
       </c>
       <c r="C6">
-        <f>9.8*B6</f>
+        <f t="shared" si="9"/>
         <v>89.434799999999996</v>
       </c>
       <c r="D6">
         <v>72</v>
       </c>
       <c r="E6">
-        <f>D6/1000 *25.4</f>
+        <f t="shared" si="10"/>
         <v>1.8287999999999998</v>
       </c>
       <c r="F6">
-        <f>C6/E6</f>
+        <f t="shared" si="11"/>
         <v>48.903543307086615</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <f>I2-I4</f>
+        <v>47.374638911386015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <f>A7*0.4563</f>
+        <f t="shared" si="8"/>
         <v>4.5629999999999997</v>
       </c>
       <c r="C7" s="1">
-        <f>9.8*B7</f>
+        <f t="shared" si="9"/>
         <v>44.717399999999998</v>
       </c>
       <c r="D7" s="1">
@@ -548,72 +631,86 @@
         <v>34</v>
       </c>
       <c r="E7" s="1">
-        <f>D7/1000 *25.4</f>
+        <f t="shared" si="10"/>
         <v>0.86360000000000003</v>
       </c>
       <c r="F7" s="1">
-        <f>C7/E7</f>
+        <f t="shared" si="11"/>
         <v>51.780222325150525</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4">
+        <f>197/2.5</f>
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
       <c r="B8">
-        <f>A8*0.4563</f>
+        <f t="shared" si="8"/>
         <v>4.5629999999999997</v>
       </c>
       <c r="C8">
-        <f>9.8*B8</f>
+        <f t="shared" si="9"/>
         <v>44.717399999999998</v>
       </c>
       <c r="D8">
         <v>36</v>
       </c>
       <c r="E8">
-        <f>D8/1000 *25.4</f>
+        <f t="shared" si="10"/>
         <v>0.91439999999999988</v>
       </c>
       <c r="F8">
-        <f>C8/E8</f>
+        <f t="shared" si="11"/>
         <v>48.903543307086615</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4">
+        <f>ABS(I7-I2)/I2</f>
+        <v>0.57129261145227139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20</v>
       </c>
       <c r="B9">
-        <f>A9*0.4563</f>
+        <f t="shared" si="8"/>
         <v>9.1259999999999994</v>
       </c>
       <c r="C9">
-        <f>9.8*B9</f>
+        <f t="shared" si="9"/>
         <v>89.434799999999996</v>
       </c>
       <c r="D9">
         <v>68</v>
       </c>
       <c r="E9">
-        <f>D9/1000 *25.4</f>
+        <f t="shared" si="10"/>
         <v>1.7272000000000001</v>
       </c>
       <c r="F9">
-        <f>C9/E9</f>
+        <f t="shared" si="11"/>
         <v>51.780222325150525</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <f>A10*0.4563</f>
+        <f t="shared" si="8"/>
         <v>4.5629999999999997</v>
       </c>
       <c r="C10" s="1">
-        <f>9.8*B10</f>
+        <f t="shared" si="9"/>
         <v>44.717399999999998</v>
       </c>
       <c r="D10" s="1">
@@ -621,93 +718,70 @@
         <v>32</v>
       </c>
       <c r="E10" s="1">
-        <f>D10/1000 *25.4</f>
+        <f t="shared" si="10"/>
         <v>0.81279999999999997</v>
       </c>
       <c r="F10" s="1">
-        <f>C10/E10</f>
+        <f t="shared" si="11"/>
         <v>55.016486220472437</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <f>AVERAGE(F2:F9)</f>
-        <v>49.541456915377211</v>
-      </c>
-      <c r="H12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12">
-        <f>F12+F13</f>
-        <v>53.642026272566746</v>
-      </c>
-      <c r="K12" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12">
-        <f>F12+2*F13</f>
-        <v>57.742595629756288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F13">
-        <f>_xlfn.STDEV.S(F2:F9)</f>
-        <v>4.1005693571895376</v>
-      </c>
-      <c r="H13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13">
-        <f>F12-F13</f>
-        <v>45.440887558187676</v>
-      </c>
-      <c r="K13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13">
-        <f>F12-2*F13</f>
-        <v>41.340318200998134</v>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -730,8 +804,15 @@
         <f>C2/E2</f>
         <v>60.707846863969586</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(F2:F10)</f>
+        <v>54.371103773773605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -754,8 +835,15 @@
         <f t="shared" ref="F3" si="3">C3/E3</f>
         <v>56.791211582423166</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <f>_xlfn.STDEV.S(F2:F10)</f>
+        <v>6.1811431065677231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>10</v>
       </c>
@@ -779,65 +867,86 @@
         <f t="shared" ref="F4" si="4">C4/E4</f>
         <v>53.349319971367215</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <f>_xlfn.CONFIDENCE.NORM(0.05,I3,COUNT(F2:F10))</f>
+        <v>4.0382726240535867</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5">
-        <f>A5*0.4563</f>
+        <f t="shared" ref="B5:B10" si="5">A5*0.4563</f>
         <v>4.5629999999999997</v>
       </c>
       <c r="C5">
-        <f>9.8*B5</f>
+        <f t="shared" ref="C5:C10" si="6">9.8*B5</f>
         <v>44.717399999999998</v>
       </c>
       <c r="D5">
         <v>32</v>
       </c>
       <c r="E5">
-        <f>D5/1000*25.4</f>
+        <f t="shared" ref="E5:E10" si="7">D5/1000*25.4</f>
         <v>0.81279999999999997</v>
       </c>
       <c r="F5">
-        <f>C5/E5</f>
+        <f t="shared" ref="F5:F10" si="8">C5/E5</f>
         <v>55.016486220472437</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <f>I2+I4</f>
+        <v>58.409376397827188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
       <c r="B6">
-        <f>A6*0.4563</f>
+        <f t="shared" si="5"/>
         <v>9.1259999999999994</v>
       </c>
       <c r="C6">
-        <f>9.8*B6</f>
+        <f t="shared" si="6"/>
         <v>89.434799999999996</v>
       </c>
       <c r="D6">
         <v>70.5</v>
       </c>
       <c r="E6">
-        <f>D6/1000*25.4</f>
+        <f t="shared" si="7"/>
         <v>1.7906999999999997</v>
       </c>
       <c r="F6">
-        <f>C6/E6</f>
+        <f t="shared" si="8"/>
         <v>49.944044228513995</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <f>I2-I4</f>
+        <v>50.332831149720022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <f>A7*0.4563</f>
+        <f t="shared" si="5"/>
         <v>4.5629999999999997</v>
       </c>
       <c r="C7" s="1">
-        <f>9.8*B7</f>
+        <f t="shared" si="6"/>
         <v>44.717399999999998</v>
       </c>
       <c r="D7" s="1">
@@ -845,72 +954,86 @@
         <v>38.5</v>
       </c>
       <c r="E7" s="1">
-        <f>D7/1000*25.4</f>
+        <f t="shared" si="7"/>
         <v>0.97789999999999988</v>
       </c>
       <c r="F7" s="1">
-        <f>C7/E7</f>
+        <f t="shared" si="8"/>
         <v>45.727988546886188</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4">
+        <f>197/2.7</f>
+        <v>72.962962962962962</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
       <c r="B8">
-        <f>A8*0.4563</f>
+        <f t="shared" si="5"/>
         <v>4.5629999999999997</v>
       </c>
       <c r="C8">
-        <f>9.8*B8</f>
+        <f t="shared" si="6"/>
         <v>44.717399999999998</v>
       </c>
       <c r="D8">
         <v>27</v>
       </c>
       <c r="E8">
-        <f>D8/1000*25.4</f>
+        <f t="shared" si="7"/>
         <v>0.68579999999999997</v>
       </c>
       <c r="F8">
-        <f>C8/E8</f>
+        <f t="shared" si="8"/>
         <v>65.204724409448815</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4">
+        <f>ABS(I7-I2)/I2</f>
+        <v>0.3419437513453113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20</v>
       </c>
       <c r="B9">
-        <f>A9*0.4563</f>
+        <f t="shared" si="5"/>
         <v>9.1259999999999994</v>
       </c>
       <c r="C9">
-        <f>9.8*B9</f>
+        <f t="shared" si="6"/>
         <v>89.434799999999996</v>
       </c>
       <c r="D9">
         <v>64</v>
       </c>
       <c r="E9">
-        <f>D9/1000*25.4</f>
+        <f t="shared" si="7"/>
         <v>1.6255999999999999</v>
       </c>
       <c r="F9">
-        <f>C9/E9</f>
+        <f t="shared" si="8"/>
         <v>55.016486220472437</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <f>A10*0.4563</f>
+        <f t="shared" si="5"/>
         <v>4.5629999999999997</v>
       </c>
       <c r="C10" s="1">
-        <f>9.8*B10</f>
+        <f t="shared" si="6"/>
         <v>44.717399999999998</v>
       </c>
       <c r="D10" s="1">
@@ -918,18 +1041,18 @@
         <v>37</v>
       </c>
       <c r="E10" s="1">
-        <f>D10/1000*25.4</f>
+        <f t="shared" si="7"/>
         <v>0.93979999999999986</v>
       </c>
       <c r="F10" s="1">
-        <f>C10/E10</f>
+        <f t="shared" si="8"/>
         <v>47.581825920408605</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>